<commit_message>
adding the tafel window functionality. Added a new treeview widget instance - analysis tree, to make it reusable in future windows
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,97 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Potential [V]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CDL [F]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>b [F/mV/s]</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3.46e-08</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4.81e-07</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>druga</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2.22e-08</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2.09e-07</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>trzecia</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1.78e-08</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2.91e-07</t>
+          <t>Tafel slope [V/dec]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added functionality to analysis_tree.py, updating trafel_window.py, making slider.py use analysis_tree
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:B1"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Tafel slope [V/dec]</t>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Potential [V]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CDL [F]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>b [F/mV/s]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added inspect node to slider analyisis_tree. Changed slider.py so that inserting into the analysis tree, one can give additional info to TreeNode (aux)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,37 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Potential [V]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Potential [V]</t>
+          <t>CDL [F]</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CDL [F]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>b [F/mV/s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.25356765</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4.06e-08</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1.08e-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added treenode functionality and basic menu functionality
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Potential [V]</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>CDL [F]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>b [F/mV/s]</t>
+          <t>Analysis</t>
         </is>
       </c>
     </row>
@@ -456,17 +446,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.25356765</t>
+          <t>{'Doopa': 'dopa'}</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
-          <t>4.06e-08</t>
+          <t>{'Doopa': 'dopa'}</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
-          <t>1.08e-06</t>
+          <t xml:space="preserve">      HER_#1_#1.DTA  HER_#1_#2.DTA  HER_#1_#3.DTA  HER_#2_#1.DTA  HER_#2_#2.DTA  ...  HER_POWROT_#2_#1.DTA  HER_POWROT_#2_#2.DTA  HER_POWROT_#2_#3.DTA      mean       std
+0.01      -0.015307       -0.01532      -0.015309      -0.015348      -0.015335  ...               -0.0153             -0.015266             -0.015319 -0.015302  0.000027
+[1 rows x 14 columns]</t>
         </is>
       </c>
     </row>

</xml_diff>